<commit_message>
Added website page about creating a simple LED + pushbutton design for the Nano board using the GOWIN software.
</commit_message>
<xml_diff>
--- a/Sipeed_Tang_Nano/HDK/pinout.xlsx
+++ b/Sipeed_Tang_Nano/HDK/pinout.xlsx
@@ -346,6 +346,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -363,29 +364,34 @@
       <family val="0"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <b val="true"/>
-      <sz val="24"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF333333"/>
+      <color rgb="FFCC0000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <i val="true"/>
@@ -393,6 +399,36 @@
       <color rgb="FF808080"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF006600"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="24"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <u val="single"/>
@@ -400,56 +436,35 @@
       <color rgb="FF0000EE"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF006600"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF996600"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FFCC0000"/>
+      <color rgb="FF333333"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="11">
@@ -458,30 +473,6 @@
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFCC"/>
-        <bgColor rgb="FFCCFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCCCC"/>
-        <bgColor rgb="FFDDDDDD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCC0000"/>
-        <bgColor rgb="FF800000"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -499,6 +490,30 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFDDDDDD"/>
         <bgColor rgb="FFE6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor rgb="FFDDDDDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC0000"/>
+        <bgColor rgb="FF800000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFCCFFFF"/>
       </patternFill>
     </fill>
     <fill>
@@ -562,27 +577,69 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="12" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="13" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="15" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="15" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="14" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="5" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -593,11 +650,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -609,11 +666,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -625,27 +682,27 @@
     <cellStyle name="Currency" xfId="17" builtinId="4"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
-    <cellStyle name="Heading" xfId="20"/>
-    <cellStyle name="Heading 1" xfId="21"/>
-    <cellStyle name="Heading 2" xfId="22"/>
-    <cellStyle name="Text" xfId="23"/>
-    <cellStyle name="Note" xfId="24"/>
-    <cellStyle name="Footnote" xfId="25"/>
-    <cellStyle name="Hyperlink" xfId="26"/>
-    <cellStyle name="Status" xfId="27"/>
-    <cellStyle name="Good" xfId="28"/>
-    <cellStyle name="Neutral" xfId="29"/>
-    <cellStyle name="Bad" xfId="30"/>
-    <cellStyle name="Warning" xfId="31"/>
-    <cellStyle name="Error" xfId="32"/>
-    <cellStyle name="Accent" xfId="33"/>
-    <cellStyle name="Accent 1" xfId="34"/>
-    <cellStyle name="Accent 2" xfId="35"/>
-    <cellStyle name="Accent 3" xfId="36"/>
+    <cellStyle name="Accent 1 17" xfId="20"/>
+    <cellStyle name="Accent 16" xfId="21"/>
+    <cellStyle name="Accent 2 18" xfId="22"/>
+    <cellStyle name="Accent 3 19" xfId="23"/>
+    <cellStyle name="alt_yellow" xfId="24"/>
+    <cellStyle name="Bad 13" xfId="25"/>
+    <cellStyle name="Error 15" xfId="26"/>
+    <cellStyle name="Footnote 8" xfId="27"/>
+    <cellStyle name="Good 11" xfId="28"/>
+    <cellStyle name="Heading 1 4" xfId="29"/>
+    <cellStyle name="Heading 2 5" xfId="30"/>
+    <cellStyle name="Heading 3" xfId="31"/>
+    <cellStyle name="Hyperlink 9" xfId="32"/>
+    <cellStyle name="Neutral 12" xfId="33"/>
+    <cellStyle name="Note 7" xfId="34"/>
+    <cellStyle name="Status 10" xfId="35"/>
+    <cellStyle name="Text 6" xfId="36"/>
     <cellStyle name="Untitled1" xfId="37"/>
     <cellStyle name="Untitled2" xfId="38"/>
     <cellStyle name="Untitled3" xfId="39"/>
-    <cellStyle name="alt_yellow" xfId="40"/>
+    <cellStyle name="Warning 14" xfId="40"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -744,9 +801,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>104760</xdr:colOff>
+      <xdr:colOff>104040</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>143640</xdr:rowOff>
+      <xdr:rowOff>142920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -759,8 +816,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10190160" y="344520"/>
-          <a:ext cx="6430680" cy="7777080"/>
+          <a:off x="10189440" y="344520"/>
+          <a:ext cx="6429960" cy="7776360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -782,7 +839,7 @@
   </sheetPr>
   <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J52" activeCellId="0" sqref="J52"/>
     </sheetView>
   </sheetViews>
@@ -791,11 +848,11 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.31"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="6" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="13.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="14.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="14.88"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="11.52"/>
   </cols>
   <sheetData>

</xml_diff>